<commit_message>
Updates for 3.3.1 (minus WebAppData)
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
+++ b/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/TARGET_eps-us-3.2.1/InputData/zzz_ccs/BFoCPAbS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-mexico\InputData\ccs\BFoCPAbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB034F63-3815-6D4B-A3A8-38504CE1DA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752E5E80-4CF4-45CA-9E32-743365988702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="33360" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Global CCS Database" sheetId="13" r:id="rId2"/>
     <sheet name="BAU Calculations" sheetId="14" r:id="rId3"/>
     <sheet name="BFoCPAbS-electricity" sheetId="15" r:id="rId4"/>
-    <sheet name="BFoCPAbS-industry" sheetId="16" r:id="rId5"/>
+    <sheet name="BFoCPAbS-industry-energyEmis" sheetId="16" r:id="rId5"/>
+    <sheet name="BFoCPAbS-industry-processEmis" sheetId="17" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Global CCS Database'!$A$7:$K$36</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="186">
   <si>
     <t>Source:</t>
   </si>
@@ -793,7 +794,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -816,7 +817,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -872,7 +873,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-MX"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2147,7 +2148,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MX"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2086371983"/>
@@ -2203,7 +2204,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MX"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2095671583"/>
@@ -2242,7 +2243,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-MX"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2283,7 +2284,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-MX"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2297,7 +2298,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2359,7 +2360,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-MX"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3667,7 +3668,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MX"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1719908479"/>
@@ -3726,7 +3727,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MX"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2086375631"/>
@@ -3768,7 +3769,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-MX"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3805,7 +3806,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-MX"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3819,7 +3820,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3881,7 +3882,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-MX"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5189,7 +5190,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MX"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1791667823"/>
@@ -5248,7 +5249,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-MX"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1947137231"/>
@@ -5290,7 +5291,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-MX"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5327,7 +5328,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-MX"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7446,20 +7447,20 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="103.5" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="103.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7467,50 +7468,50 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="31">
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>183</v>
       </c>
@@ -7519,7 +7520,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>184</v>
       </c>
@@ -7528,26 +7529,26 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
@@ -7566,46 +7567,46 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="86.5" customWidth="1"/>
-    <col min="9" max="9" width="10.1640625" style="22" customWidth="1"/>
-    <col min="10" max="10" width="25.5" style="9" customWidth="1"/>
-    <col min="11" max="11" width="37.5" style="9" customWidth="1"/>
+    <col min="7" max="7" width="86.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="37.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -7640,7 +7641,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
@@ -7673,7 +7674,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
@@ -7709,7 +7710,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>29</v>
       </c>
@@ -7742,7 +7743,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>31</v>
       </c>
@@ -7775,7 +7776,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>34</v>
       </c>
@@ -7811,7 +7812,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>36</v>
       </c>
@@ -7844,7 +7845,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>38</v>
       </c>
@@ -7876,7 +7877,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>43</v>
       </c>
@@ -7912,7 +7913,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>46</v>
       </c>
@@ -7944,7 +7945,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>50</v>
       </c>
@@ -7977,7 +7978,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>52</v>
       </c>
@@ -8013,7 +8014,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>54</v>
       </c>
@@ -8046,7 +8047,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>57</v>
       </c>
@@ -8079,7 +8080,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>59</v>
       </c>
@@ -8113,7 +8114,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>61</v>
       </c>
@@ -8146,7 +8147,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>63</v>
       </c>
@@ -8179,7 +8180,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>65</v>
       </c>
@@ -8213,7 +8214,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>67</v>
       </c>
@@ -8246,7 +8247,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>70</v>
       </c>
@@ -8278,7 +8279,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>74</v>
       </c>
@@ -8311,7 +8312,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>76</v>
       </c>
@@ -8344,7 +8345,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>78</v>
       </c>
@@ -8376,7 +8377,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>81</v>
       </c>
@@ -8410,7 +8411,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>83</v>
       </c>
@@ -8443,7 +8444,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>85</v>
       </c>
@@ -8479,7 +8480,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>88</v>
       </c>
@@ -8512,7 +8513,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>90</v>
       </c>
@@ -8543,7 +8544,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>92</v>
       </c>
@@ -8576,7 +8577,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>94</v>
       </c>
@@ -8624,13 +8625,13 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.5" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>101</v>
       </c>
@@ -8668,7 +8669,7 @@
       <c r="AG1" s="7"/>
       <c r="AH1" s="7"/>
     </row>
-    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="33">
         <v>2018</v>
@@ -8770,7 +8771,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>116</v>
       </c>
@@ -8907,7 +8908,7 @@
         <v>6400000</v>
       </c>
     </row>
-    <row r="4" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>117</v>
       </c>
@@ -9044,7 +9045,7 @@
         <v>1400000</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>164</v>
       </c>
@@ -9181,7 +9182,7 @@
         <v>1490000</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>165</v>
       </c>
@@ -9318,7 +9319,7 @@
         <v>7575000</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>178</v>
       </c>
@@ -9455,66 +9456,66 @@
         <v>23138095.238095239</v>
       </c>
     </row>
-    <row r="8" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
     </row>
-    <row r="17" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
     </row>
-    <row r="18" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
     </row>
-    <row r="27" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
       <c r="B32" s="33">
         <v>2018</v>
@@ -9616,7 +9617,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="33" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
         <v>116</v>
       </c>
@@ -9720,7 +9721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
         <v>117</v>
       </c>
@@ -9824,7 +9825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
         <v>164</v>
       </c>
@@ -9928,7 +9929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>165</v>
       </c>
@@ -10032,7 +10033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:34" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>178</v>
       </c>
@@ -10136,55 +10137,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
     </row>
-    <row r="39" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
     </row>
-    <row r="40" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
     </row>
-    <row r="41" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
     </row>
-    <row r="42" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
     </row>
-    <row r="43" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
     </row>
-    <row r="44" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
     </row>
-    <row r="45" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
     </row>
-    <row r="46" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
     </row>
-    <row r="47" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
     </row>
-    <row r="48" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17"/>
     </row>
-    <row r="49" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
     </row>
-    <row r="50" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
     </row>
-    <row r="51" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17"/>
     </row>
-    <row r="52" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17"/>
     </row>
-    <row r="53" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17"/>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>149</v>
       </c>
@@ -10222,12 +10223,12 @@
       <c r="AG55" s="7"/>
       <c r="AH55" s="7"/>
     </row>
-    <row r="56" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>100</v>
       </c>
@@ -10328,7 +10329,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="58" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>133</v>
       </c>
@@ -10429,7 +10430,7 @@
         <v>957155000000000</v>
       </c>
     </row>
-    <row r="59" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>134</v>
       </c>
@@ -10530,7 +10531,7 @@
         <v>344835000000000</v>
       </c>
     </row>
-    <row r="60" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>135</v>
       </c>
@@ -10631,7 +10632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>136</v>
       </c>
@@ -10732,7 +10733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>137</v>
       </c>
@@ -10833,7 +10834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>138</v>
       </c>
@@ -10934,7 +10935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>139</v>
       </c>
@@ -11035,7 +11036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>140</v>
       </c>
@@ -11136,7 +11137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>141</v>
       </c>
@@ -11237,7 +11238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>142</v>
       </c>
@@ -11338,7 +11339,7 @@
         <v>11286300000000</v>
       </c>
     </row>
-    <row r="68" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>143</v>
       </c>
@@ -11439,7 +11440,7 @@
         <v>99792600000000</v>
       </c>
     </row>
-    <row r="69" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>144</v>
       </c>
@@ -11540,7 +11541,7 @@
         <v>43507100000000</v>
       </c>
     </row>
-    <row r="70" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>145</v>
       </c>
@@ -11641,7 +11642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>146</v>
       </c>
@@ -11742,7 +11743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>147</v>
       </c>
@@ -11843,7 +11844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>148</v>
       </c>
@@ -11944,7 +11945,7 @@
         <v>24454600000000</v>
       </c>
     </row>
-    <row r="74" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="26"/>
       <c r="C74" s="26"/>
       <c r="D74" s="26"/>
@@ -11978,12 +11979,12 @@
       <c r="AF74" s="26"/>
       <c r="AG74" s="26"/>
     </row>
-    <row r="75" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="76" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>100</v>
       </c>
@@ -12084,7 +12085,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="77" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>150</v>
       </c>
@@ -12185,7 +12186,7 @@
         <v>455116000000000</v>
       </c>
     </row>
-    <row r="78" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>151</v>
       </c>
@@ -12286,7 +12287,7 @@
         <v>400057000000000</v>
       </c>
     </row>
-    <row r="80" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>102</v>
       </c>
@@ -12324,7 +12325,7 @@
       <c r="AG80" s="7"/>
       <c r="AH80" s="7"/>
     </row>
-    <row r="81" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="20"/>
       <c r="B81">
         <v>2019</v>
@@ -12423,7 +12424,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="82" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
         <v>116</v>
       </c>
@@ -12556,7 +12557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
         <v>117</v>
       </c>
@@ -12689,7 +12690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:33" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="28" t="s">
         <v>164</v>
       </c>
@@ -12822,7 +12823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:33" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="28" t="s">
         <v>165</v>
       </c>
@@ -12955,7 +12956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:33" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
         <v>178</v>
       </c>
@@ -13088,100 +13089,100 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="20"/>
     </row>
-    <row r="88" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="20"/>
     </row>
-    <row r="89" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="20"/>
     </row>
-    <row r="90" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="20"/>
     </row>
-    <row r="91" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="20"/>
     </row>
-    <row r="92" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="20"/>
     </row>
-    <row r="93" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="20"/>
     </row>
-    <row r="94" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
     </row>
-    <row r="95" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="20"/>
     </row>
-    <row r="96" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:33" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="20"/>
     </row>
-    <row r="97" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="20"/>
     </row>
-    <row r="98" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="20"/>
     </row>
-    <row r="99" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="20"/>
     </row>
-    <row r="100" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="20"/>
     </row>
-    <row r="101" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="20"/>
     </row>
-    <row r="102" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="20"/>
     </row>
-    <row r="103" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="20"/>
     </row>
-    <row r="104" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="20"/>
     </row>
-    <row r="105" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="20"/>
     </row>
-    <row r="106" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="20"/>
     </row>
-    <row r="107" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="20"/>
     </row>
-    <row r="108" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="20"/>
     </row>
-    <row r="109" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="110" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="112" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
         <v>113</v>
       </c>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>2019</v>
       </c>
@@ -13189,7 +13190,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="27" t="s">
         <v>116</v>
       </c>
@@ -13202,7 +13203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="27" t="s">
         <v>117</v>
       </c>
@@ -13215,7 +13216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="28" t="s">
         <v>164</v>
       </c>
@@ -13231,7 +13232,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="28" t="s">
         <v>165</v>
       </c>
@@ -13244,7 +13245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="28" t="s">
         <v>178</v>
       </c>
@@ -13275,12 +13276,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.83203125" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>115</v>
       </c>
@@ -13381,7 +13382,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>116</v>
       </c>
@@ -13514,7 +13515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>117</v>
       </c>
@@ -13647,7 +13648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>125</v>
       </c>
@@ -13748,7 +13749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>126</v>
       </c>
@@ -13849,7 +13850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>127</v>
       </c>
@@ -13950,7 +13951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>128</v>
       </c>
@@ -14051,7 +14052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>129</v>
       </c>
@@ -14152,7 +14153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>118</v>
       </c>
@@ -14253,7 +14254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>130</v>
       </c>
@@ -14354,7 +14355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>119</v>
       </c>
@@ -14455,7 +14456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>120</v>
       </c>
@@ -14556,7 +14557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>121</v>
       </c>
@@ -14657,7 +14658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>131</v>
       </c>
@@ -14758,7 +14759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>122</v>
       </c>
@@ -14859,7 +14860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>123</v>
       </c>
@@ -14960,7 +14961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>124</v>
       </c>
@@ -15078,12 +15079,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.83203125" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>115</v>
       </c>
@@ -15184,7 +15185,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>156</v>
       </c>
@@ -15285,7 +15286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -15386,7 +15387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>158</v>
       </c>
@@ -15487,7 +15488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>159</v>
       </c>
@@ -15588,7 +15589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -15689,7 +15690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -15790,7 +15791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -15891,7 +15892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -15992,7 +15993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -16125,7 +16126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -16258,7 +16259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -16359,7 +16360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -16460,7 +16461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>168</v>
       </c>
@@ -16561,7 +16562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>169</v>
       </c>
@@ -16662,7 +16663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>170</v>
       </c>
@@ -16763,7 +16764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>171</v>
       </c>
@@ -16864,7 +16865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -16965,7 +16966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>173</v>
       </c>
@@ -17066,7 +17067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>174</v>
       </c>
@@ -17167,7 +17168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>175</v>
       </c>
@@ -17268,7 +17269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>176</v>
       </c>
@@ -17369,7 +17370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>177</v>
       </c>
@@ -17470,7 +17471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>178</v>
       </c>
@@ -17603,7 +17604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>179</v>
       </c>
@@ -17704,7 +17705,2751 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AG26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F3D46E-7449-4A44-9543-8C97370F914F}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:AG26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2035</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2036</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2037</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2038</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2039</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2040</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2041</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2042</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2043</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>2044</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" cm="1">
+        <f t="array" ref="B10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" cm="1">
+        <f t="array" ref="C10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,C$1)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" cm="1">
+        <f t="array" ref="D10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" cm="1">
+        <f t="array" ref="E10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" cm="1">
+        <f t="array" ref="F10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,F$1)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" cm="1">
+        <f t="array" ref="G10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,G$1)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" cm="1">
+        <f t="array" ref="H10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,H$1)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" cm="1">
+        <f t="array" ref="I10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" cm="1">
+        <f t="array" ref="J10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" cm="1">
+        <f t="array" ref="K10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" cm="1">
+        <f t="array" ref="L10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" cm="1">
+        <f t="array" ref="M10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" cm="1">
+        <f t="array" ref="N10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,N$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O10" cm="1">
+        <f t="array" ref="O10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,O$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" cm="1">
+        <f t="array" ref="P10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,P$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" cm="1">
+        <f t="array" ref="Q10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,Q$1)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" cm="1">
+        <f t="array" ref="R10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,R$1)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" cm="1">
+        <f t="array" ref="S10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,S$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T10" cm="1">
+        <f t="array" ref="T10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,T$1)</f>
+        <v>0</v>
+      </c>
+      <c r="U10" cm="1">
+        <f t="array" ref="U10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,U$1)</f>
+        <v>0</v>
+      </c>
+      <c r="V10" cm="1">
+        <f t="array" ref="V10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,V$1)</f>
+        <v>0</v>
+      </c>
+      <c r="W10" cm="1">
+        <f t="array" ref="W10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,W$1)</f>
+        <v>0</v>
+      </c>
+      <c r="X10" cm="1">
+        <f t="array" ref="X10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,X$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y10" cm="1">
+        <f t="array" ref="Y10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,Y$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Z10" cm="1">
+        <f t="array" ref="Z10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,Z$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AA10" cm="1">
+        <f t="array" ref="AA10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,AA$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AB10" cm="1">
+        <f t="array" ref="AB10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,AB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AC10" cm="1">
+        <f t="array" ref="AC10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,AC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AD10" cm="1">
+        <f t="array" ref="AD10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,AD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AE10" cm="1">
+        <f t="array" ref="AE10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,AE$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AF10" cm="1">
+        <f t="array" ref="AF10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,AF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AG10" cm="1">
+        <f t="array" ref="AG10">TREND('BAU Calculations'!$B118:$C118,'BAU Calculations'!$B$115:$C$115,AG$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" cm="1">
+        <f t="array" ref="B11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" cm="1">
+        <f t="array" ref="C11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,C$1)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" cm="1">
+        <f t="array" ref="D11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" cm="1">
+        <f t="array" ref="E11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" cm="1">
+        <f t="array" ref="F11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,F$1)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" cm="1">
+        <f t="array" ref="G11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,G$1)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" cm="1">
+        <f t="array" ref="H11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,H$1)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" cm="1">
+        <f t="array" ref="I11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" cm="1">
+        <f t="array" ref="J11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" cm="1">
+        <f t="array" ref="K11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" cm="1">
+        <f t="array" ref="L11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" cm="1">
+        <f t="array" ref="M11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" cm="1">
+        <f t="array" ref="N11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,N$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O11" cm="1">
+        <f t="array" ref="O11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,O$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" cm="1">
+        <f t="array" ref="P11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,P$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" cm="1">
+        <f t="array" ref="Q11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,Q$1)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" cm="1">
+        <f t="array" ref="R11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,R$1)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" cm="1">
+        <f t="array" ref="S11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,S$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" cm="1">
+        <f t="array" ref="T11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,T$1)</f>
+        <v>0</v>
+      </c>
+      <c r="U11" cm="1">
+        <f t="array" ref="U11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,U$1)</f>
+        <v>0</v>
+      </c>
+      <c r="V11" cm="1">
+        <f t="array" ref="V11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,V$1)</f>
+        <v>0</v>
+      </c>
+      <c r="W11" cm="1">
+        <f t="array" ref="W11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,W$1)</f>
+        <v>0</v>
+      </c>
+      <c r="X11" cm="1">
+        <f t="array" ref="X11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,X$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" cm="1">
+        <f t="array" ref="Y11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,Y$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" cm="1">
+        <f t="array" ref="Z11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,Z$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AA11" cm="1">
+        <f t="array" ref="AA11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,AA$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AB11" cm="1">
+        <f t="array" ref="AB11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,AB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AC11" cm="1">
+        <f t="array" ref="AC11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,AC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AD11" cm="1">
+        <f t="array" ref="AD11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,AD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AE11" cm="1">
+        <f t="array" ref="AE11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,AE$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AF11" cm="1">
+        <f t="array" ref="AF11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,AF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AG11" cm="1">
+        <f t="array" ref="AG11">TREND('BAU Calculations'!$B119:$C119,'BAU Calculations'!$B$115:$C$115,AG$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" cm="1">
+        <f t="array" ref="B24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" cm="1">
+        <f t="array" ref="C24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,C$1)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" cm="1">
+        <f t="array" ref="D24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" cm="1">
+        <f t="array" ref="E24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" cm="1">
+        <f t="array" ref="F24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,F$1)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" cm="1">
+        <f t="array" ref="G24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,G$1)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" cm="1">
+        <f t="array" ref="H24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,H$1)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" cm="1">
+        <f t="array" ref="I24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" cm="1">
+        <f t="array" ref="J24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" cm="1">
+        <f t="array" ref="K24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L24" cm="1">
+        <f t="array" ref="L24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" cm="1">
+        <f t="array" ref="M24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" cm="1">
+        <f t="array" ref="N24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,N$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O24" cm="1">
+        <f t="array" ref="O24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,O$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P24" cm="1">
+        <f t="array" ref="P24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,P$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" cm="1">
+        <f t="array" ref="Q24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,Q$1)</f>
+        <v>0</v>
+      </c>
+      <c r="R24" cm="1">
+        <f t="array" ref="R24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,R$1)</f>
+        <v>0</v>
+      </c>
+      <c r="S24" cm="1">
+        <f t="array" ref="S24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,S$1)</f>
+        <v>0</v>
+      </c>
+      <c r="T24" cm="1">
+        <f t="array" ref="T24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,T$1)</f>
+        <v>0</v>
+      </c>
+      <c r="U24" cm="1">
+        <f t="array" ref="U24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,U$1)</f>
+        <v>0</v>
+      </c>
+      <c r="V24" cm="1">
+        <f t="array" ref="V24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,V$1)</f>
+        <v>0</v>
+      </c>
+      <c r="W24" cm="1">
+        <f t="array" ref="W24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,W$1)</f>
+        <v>0</v>
+      </c>
+      <c r="X24" cm="1">
+        <f t="array" ref="X24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,X$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y24" cm="1">
+        <f t="array" ref="Y24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,Y$1)</f>
+        <v>0</v>
+      </c>
+      <c r="Z24" cm="1">
+        <f t="array" ref="Z24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,Z$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AA24" cm="1">
+        <f t="array" ref="AA24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,AA$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AB24" cm="1">
+        <f t="array" ref="AB24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,AB$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AC24" cm="1">
+        <f t="array" ref="AC24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,AC$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AD24" cm="1">
+        <f t="array" ref="AD24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,AD$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AE24" cm="1">
+        <f t="array" ref="AE24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,AE$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AF24" cm="1">
+        <f t="array" ref="AF24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,AF$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AG24" cm="1">
+        <f t="array" ref="AG24">TREND('BAU Calculations'!$B120:$C120,'BAU Calculations'!$B$115:$C$115,AG$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>180</v>
       </c>

</xml_diff>